<commit_message>
created linked and sensitivity versions of model (work in progress) and versions of model with alternative business models.
The alternative business models change the benefits of the NPV formulations. Demand Charge has the benefit of the electricity that can be directly used from the panels (instead of all of the electricity that is generated by the panels, which is the benefit under a net-metering system). WholesaleComp uses the wholesale price of electricity to compensate PV customers.

The import sheet has also been extensively updated, especially the sensitivity variables. Still need to whittle these down to make a reasonable number of evaluation cases.
</commit_message>
<xml_diff>
--- a/Model/Data/import.xlsx
+++ b/Model/Data/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-37740" yWindow="-7700" windowWidth="36320" windowHeight="20840" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-35260" yWindow="-7700" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sydney (incomplete)" sheetId="5" r:id="rId3"/>
     <sheet name="sensitivity" sheetId="3" r:id="rId4"/>
     <sheet name="all_variables" sheetId="2" r:id="rId5"/>
+    <sheet name="Demand Charge" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -908,7 +909,7 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -929,6 +930,30 @@
           </rPr>
           <t xml:space="preserve">
 manual sensitivity analyses show that LA is highly sensitive to this value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LA value</t>
         </r>
       </text>
     </comment>
@@ -937,7 +962,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
   <si>
     <t>population growth rate</t>
   </si>
@@ -1435,6 +1460,27 @@
   </si>
   <si>
     <t>default value:</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>Retail Price</t>
+  </si>
+  <si>
+    <t>Bass flows</t>
+  </si>
+  <si>
+    <t>New homes</t>
+  </si>
+  <si>
+    <t>direct PV use</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Boulder</t>
   </si>
 </sst>
 </file>
@@ -1521,7 +1567,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1540,6 +1586,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1550,7 +1614,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1635,8 +1699,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1759,8 +1828,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1843,6 +1925,11 @@
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3673,8 +3760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3803,10 +3890,10 @@
         <v>39255.300000000003</v>
       </c>
       <c r="K2" s="50">
-        <v>42494.92</v>
+        <v>66571.504000000001</v>
       </c>
       <c r="L2" s="50">
-        <v>80061.820000000007</v>
+        <v>104138.40400000001</v>
       </c>
       <c r="M2" s="18">
         <v>300</v>
@@ -3863,10 +3950,10 @@
         <v>35888.700000000004</v>
       </c>
       <c r="K3" s="48">
-        <v>37756.68</v>
+        <v>59768.415999999997</v>
       </c>
       <c r="L3" s="48">
-        <v>72101.78</v>
+        <v>94113.516000000003</v>
       </c>
       <c r="M3" s="19">
         <v>300</v>
@@ -3923,10 +4010,10 @@
         <v>34884.300000000003</v>
       </c>
       <c r="K4" s="48">
-        <v>34450.519999999997</v>
+        <v>55846.224000000002</v>
       </c>
       <c r="L4" s="48">
-        <v>67834.420000000013</v>
+        <v>89230.124000000011</v>
       </c>
       <c r="M4" s="20">
         <v>300</v>
@@ -3983,10 +4070,10 @@
         <v>32698.800000000003</v>
       </c>
       <c r="K5" s="48">
-        <v>32378.32</v>
+        <v>52433.583999999995</v>
       </c>
       <c r="L5" s="48">
-        <v>63670.720000000001</v>
+        <v>83725.983999999997</v>
       </c>
       <c r="M5" s="20">
         <v>300</v>
@@ -4044,10 +4131,10 @@
         <v>31182.9</v>
       </c>
       <c r="K6" s="49">
-        <v>30343.56</v>
+        <v>49469.072</v>
       </c>
       <c r="L6" s="49">
-        <v>60185.260000000009</v>
+        <v>79310.772000000012</v>
       </c>
       <c r="M6" s="21">
         <v>300</v>
@@ -4105,10 +4192,10 @@
         <v>29332.2</v>
       </c>
       <c r="K7" s="49">
-        <v>28485.08</v>
+        <v>46475.495999999999</v>
       </c>
       <c r="L7" s="49">
-        <v>56555.68</v>
+        <v>74546.09599999999</v>
       </c>
       <c r="M7" s="22">
         <v>300</v>
@@ -4158,10 +4245,10 @@
         <v>28160.400000000001</v>
       </c>
       <c r="K8" s="49">
-        <v>26924.560000000001</v>
+        <v>44196.271999999997</v>
       </c>
       <c r="L8" s="49">
-        <v>53873.760000000009</v>
+        <v>71145.471999999994</v>
       </c>
       <c r="M8" s="18">
         <v>300</v>
@@ -4214,10 +4301,10 @@
         <v>27146.7</v>
       </c>
       <c r="K9" s="49">
-        <v>25307.88</v>
+        <v>41957.856</v>
       </c>
       <c r="L9" s="49">
-        <v>51286.98</v>
+        <v>67936.955999999991</v>
       </c>
       <c r="M9" s="18">
         <v>300</v>
@@ -4267,10 +4354,10 @@
         <v>26142.300000000003</v>
       </c>
       <c r="K10" s="49">
-        <v>23626.720000000001</v>
+        <v>39660.664000000004</v>
       </c>
       <c r="L10" s="49">
-        <v>48644.62</v>
+        <v>64678.564000000006</v>
       </c>
       <c r="M10" s="18">
         <v>300</v>
@@ -4320,10 +4407,10 @@
         <v>24793.800000000003</v>
       </c>
       <c r="K11" s="49">
-        <v>22511.32</v>
+        <v>37718.183999999994</v>
       </c>
       <c r="L11" s="49">
-        <v>46238.720000000001</v>
+        <v>61445.583999999995</v>
       </c>
       <c r="M11" s="18">
         <v>300</v>
@@ -4373,10 +4460,10 @@
         <v>24291.600000000002</v>
       </c>
       <c r="K12" s="49">
-        <v>21508.240000000002</v>
+        <v>36407.087999999996</v>
       </c>
       <c r="L12" s="49">
-        <v>44755.040000000001</v>
+        <v>59653.887999999992</v>
       </c>
       <c r="M12" s="18">
         <v>300</v>
@@ -4423,10 +4510,10 @@
         <v>23622</v>
       </c>
       <c r="K13" s="49">
-        <v>20170.8</v>
+        <v>34658.959999999999</v>
       </c>
       <c r="L13" s="49">
-        <v>42776.800000000003</v>
+        <v>57264.959999999999</v>
       </c>
       <c r="M13" s="18">
         <v>300</v>
@@ -4459,10 +4546,10 @@
         <v>22775.7</v>
       </c>
       <c r="K14" s="49">
-        <v>18823.48</v>
+        <v>32792.576000000001</v>
       </c>
       <c r="L14" s="49">
-        <v>40619.58</v>
+        <v>54588.675999999999</v>
       </c>
       <c r="M14" s="18">
         <v>300</v>
@@ -4494,10 +4581,10 @@
         <v>22943.100000000002</v>
       </c>
       <c r="K15" s="49">
-        <v>17792.84</v>
+        <v>31864.608</v>
       </c>
       <c r="L15" s="49">
-        <v>39749.14</v>
+        <v>53820.907999999996</v>
       </c>
       <c r="M15" s="18">
         <v>300</v>
@@ -4526,10 +4613,10 @@
         <v>22775.7</v>
       </c>
       <c r="K16" s="49">
-        <v>17068.48</v>
+        <v>31037.575999999997</v>
       </c>
       <c r="L16" s="49">
-        <v>38864.58</v>
+        <v>52833.675999999999</v>
       </c>
       <c r="M16" s="18">
         <v>300</v>
@@ -4558,10 +4645,10 @@
         <v>22608.300000000003</v>
       </c>
       <c r="K17" s="49">
-        <v>16279.12</v>
+        <v>30145.544000000002</v>
       </c>
       <c r="L17" s="49">
-        <v>37915.020000000004</v>
+        <v>51781.444000000003</v>
       </c>
       <c r="M17" s="18">
         <v>300</v>
@@ -4590,10 +4677,10 @@
         <v>22440.9</v>
       </c>
       <c r="K18" s="49">
-        <v>15749.76</v>
+        <v>29513.511999999995</v>
       </c>
       <c r="L18" s="49">
-        <v>37225.460000000006</v>
+        <v>50989.212</v>
       </c>
       <c r="M18" s="18">
         <v>300</v>
@@ -4622,10 +4709,10 @@
         <v>22273.5</v>
       </c>
       <c r="K19" s="49">
-        <v>15610.4</v>
+        <v>29271.479999999996</v>
       </c>
       <c r="L19" s="49">
-        <v>36925.9</v>
+        <v>50586.979999999996</v>
       </c>
       <c r="M19" s="18">
         <v>300</v>
@@ -4654,10 +4741,10 @@
         <v>22134</v>
       </c>
       <c r="K20" s="49">
-        <v>15537.6</v>
+        <v>29113.119999999995</v>
       </c>
       <c r="L20" s="49">
-        <v>36719.599999999999</v>
+        <v>50295.119999999995</v>
       </c>
       <c r="M20" s="18">
         <v>300</v>
@@ -4686,10 +4773,10 @@
         <v>21938.7</v>
       </c>
       <c r="K21" s="49">
-        <v>15201.68</v>
+        <v>28657.415999999997</v>
       </c>
       <c r="L21" s="49">
-        <v>36196.780000000006</v>
+        <v>49652.515999999996</v>
       </c>
       <c r="M21" s="18">
         <v>300</v>
@@ -4718,10 +4805,10 @@
         <v>21483</v>
       </c>
       <c r="K22" s="49">
-        <v>14981.2</v>
+        <v>28157.439999999999</v>
       </c>
       <c r="L22" s="49">
-        <v>35540.199999999997</v>
+        <v>48716.44</v>
       </c>
       <c r="M22" s="18">
         <v>300</v>
@@ -4750,10 +4837,10 @@
         <v>21269.100000000002</v>
       </c>
       <c r="K23" s="49">
-        <v>14904.24</v>
+        <v>27949.288</v>
       </c>
       <c r="L23" s="49">
-        <v>35258.54</v>
+        <v>48303.588000000003</v>
       </c>
       <c r="M23" s="18">
         <v>300</v>
@@ -4776,10 +4863,10 @@
         <v>21204</v>
       </c>
       <c r="K24" s="49">
-        <v>14835.6</v>
+        <v>27840.719999999998</v>
       </c>
       <c r="L24" s="49">
-        <v>35127.599999999999</v>
+        <v>48132.72</v>
       </c>
       <c r="M24" s="18">
         <v>300</v>
@@ -4802,10 +4889,10 @@
         <v>21166.800000000003</v>
       </c>
       <c r="K25" s="49">
-        <v>14768.52</v>
+        <v>27750.824000000001</v>
       </c>
       <c r="L25" s="49">
-        <v>35024.920000000006</v>
+        <v>48007.224000000002</v>
       </c>
       <c r="M25" s="18">
         <v>300</v>
@@ -4828,10 +4915,10 @@
         <v>21129.600000000002</v>
       </c>
       <c r="K26" s="49">
-        <v>14701.44</v>
+        <v>27660.928</v>
       </c>
       <c r="L26" s="49">
-        <v>34922.239999999998</v>
+        <v>47881.728000000003</v>
       </c>
       <c r="M26" s="18">
         <v>300</v>
@@ -4854,10 +4941,10 @@
         <v>21092.400000000001</v>
       </c>
       <c r="K27" s="49">
-        <v>14569.36</v>
+        <v>27506.031999999999</v>
       </c>
       <c r="L27" s="49">
-        <v>34754.560000000005</v>
+        <v>47691.232000000004</v>
       </c>
       <c r="M27" s="18">
         <v>300</v>
@@ -4880,10 +4967,10 @@
         <v>21055.200000000001</v>
       </c>
       <c r="K28" s="49">
-        <v>14437.279999999999</v>
+        <v>27351.135999999995</v>
       </c>
       <c r="L28" s="49">
-        <v>34586.879999999997</v>
+        <v>47500.735999999997</v>
       </c>
       <c r="M28" s="18">
         <v>300</v>
@@ -4906,10 +4993,10 @@
         <v>21018</v>
       </c>
       <c r="K29" s="49">
-        <v>14240.2</v>
+        <v>27131.239999999998</v>
       </c>
       <c r="L29" s="49">
-        <v>34354.199999999997</v>
+        <v>47245.24</v>
       </c>
       <c r="M29" s="18">
         <v>300</v>
@@ -4932,10 +5019,10 @@
         <v>20980.800000000003</v>
       </c>
       <c r="K30" s="49">
-        <v>14173.119999999999</v>
+        <v>27041.343999999997</v>
       </c>
       <c r="L30" s="49">
-        <v>34251.519999999997</v>
+        <v>47119.743999999999</v>
       </c>
       <c r="M30" s="18">
         <v>300</v>
@@ -4958,10 +5045,10 @@
         <v>20943.600000000002</v>
       </c>
       <c r="K31" s="49">
-        <v>14106.04</v>
+        <v>26951.447999999997</v>
       </c>
       <c r="L31" s="49">
-        <v>34148.839999999997</v>
+        <v>46994.247999999992</v>
       </c>
       <c r="M31" s="18">
         <v>300</v>
@@ -4984,10 +5071,10 @@
         <v>20906.400000000001</v>
       </c>
       <c r="K32" s="49">
-        <v>13973.960000000001</v>
+        <v>26796.552</v>
       </c>
       <c r="L32" s="49">
-        <v>33981.160000000003</v>
+        <v>46803.752000000008</v>
       </c>
       <c r="M32" s="18">
         <v>300</v>
@@ -5010,10 +5097,10 @@
         <v>20869.2</v>
       </c>
       <c r="K33" s="49">
-        <v>13776.880000000001</v>
+        <v>26576.655999999999</v>
       </c>
       <c r="L33" s="49">
-        <v>33748.480000000003</v>
+        <v>46548.256000000001</v>
       </c>
       <c r="M33" s="18">
         <v>300</v>
@@ -5036,10 +5123,10 @@
         <v>20832</v>
       </c>
       <c r="K34" s="49">
-        <v>13644.8</v>
+        <v>26421.759999999995</v>
       </c>
       <c r="L34" s="49">
-        <v>33580.800000000003</v>
+        <v>46357.759999999995</v>
       </c>
       <c r="M34" s="18">
         <v>300</v>
@@ -5062,10 +5149,10 @@
         <v>20794.800000000003</v>
       </c>
       <c r="K35" s="49">
-        <v>13577.720000000001</v>
+        <v>26331.864000000001</v>
       </c>
       <c r="L35" s="49">
-        <v>33478.120000000003</v>
+        <v>46232.264000000003</v>
       </c>
       <c r="M35" s="18">
         <v>300</v>
@@ -5088,10 +5175,10 @@
         <v>20757.600000000002</v>
       </c>
       <c r="K36" s="49">
-        <v>13510.64</v>
+        <v>26241.967999999997</v>
       </c>
       <c r="L36" s="49">
-        <v>33375.440000000002</v>
+        <v>46106.767999999996</v>
       </c>
       <c r="M36" s="18">
         <v>300</v>
@@ -5114,10 +5201,10 @@
         <v>20720.400000000001</v>
       </c>
       <c r="K37" s="49">
-        <v>13443.56</v>
+        <v>26152.071999999996</v>
       </c>
       <c r="L37" s="49">
-        <v>33272.76</v>
+        <v>45981.271999999997</v>
       </c>
       <c r="M37" s="18">
         <v>300</v>
@@ -5140,10 +5227,10 @@
         <v>20683.2</v>
       </c>
       <c r="K38" s="49">
-        <v>13376.48</v>
+        <v>26062.175999999999</v>
       </c>
       <c r="L38" s="49">
-        <v>33170.080000000002</v>
+        <v>45855.776000000005</v>
       </c>
       <c r="M38" s="18">
         <v>300</v>
@@ -5186,149 +5273,149 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="22" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="14.5" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="37" customFormat="1" ht="90">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="J1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="K1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="N1" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="O1" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="P1" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="Q1" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="R1" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="T1" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="U1" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="R1" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="S1" s="15" t="s">
+      <c r="V1" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="W1" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="X1" s="58" t="s">
         <v>143</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
         <v>165</v>
       </c>
-      <c r="B2">
-        <v>0.5</v>
+      <c r="B2" s="33">
+        <v>0</v>
       </c>
       <c r="C2" s="33">
         <v>0</v>
       </c>
-      <c r="D2" s="33">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14">
+        <v>2000000</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="8">
         <v>0.01</v>
       </c>
-      <c r="F2" s="9">
+      <c r="K2" s="14">
+        <v>1000</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="N2" s="9">
         <v>5</v>
       </c>
-      <c r="G2" s="51">
+      <c r="O2" s="51">
         <v>0.5</v>
       </c>
-      <c r="H2" s="14">
+      <c r="P2" s="14">
         <v>20</v>
-      </c>
-      <c r="I2" s="9">
-        <v>10</v>
-      </c>
-      <c r="J2" s="13">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="K2" s="9">
-        <v>1</v>
-      </c>
-      <c r="L2" s="9">
-        <v>1</v>
-      </c>
-      <c r="M2" s="9">
-        <v>1</v>
-      </c>
-      <c r="N2" s="9">
-        <v>1</v>
-      </c>
-      <c r="O2" s="9">
-        <v>1</v>
-      </c>
-      <c r="P2" s="9">
-        <v>1</v>
       </c>
       <c r="Q2" s="9">
         <v>10</v>
       </c>
-      <c r="R2" s="14">
-        <v>2000000</v>
-      </c>
-      <c r="S2" s="9">
-        <v>2</v>
+      <c r="R2" s="9">
+        <v>10</v>
+      </c>
+      <c r="S2" s="13">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="T2" s="9">
         <v>1</v>
@@ -5337,49 +5424,69 @@
         <v>1</v>
       </c>
       <c r="V2" s="9">
-        <v>0.01</v>
+        <v>2</v>
       </c>
       <c r="W2" s="9">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="X2" s="9">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:24">
+      <c r="B3" s="9"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="J3" s="13"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:24">
+      <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" spans="1:24">
+      <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:24">
+      <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="61" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="59" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5876,4 +5983,46 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="62">
+        <v>6211.2916123429659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="62">
+        <v>7007.1402678343975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes. added sydney values to import.xlsx
</commit_message>
<xml_diff>
--- a/Model/Data/import.xlsx
+++ b/Model/Data/import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35260" yWindow="-7700" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-35260" yWindow="-7700" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="1" r:id="rId1"/>
@@ -909,6 +909,469 @@
     <author>Nick Laws</author>
   </authors>
   <commentList>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+calibrated to produce correct fraction of utility costs from generation
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>45% for Sydney</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical, initialized with latest census value. Assumed to drop with time for LA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+see spreadsheet "FCI and LOCE forecasts Boulder"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+(graphical s-curve) 
+function of (customers_with_PV+defectors)
+/ (total_households+1)
+This function slows the rate of solar adoption as the ratio of </t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>homes with PV</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (including defectors) to</t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> total homes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> approaches  the ratio of </t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>owner occupied homes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> to </t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>total homes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>. This limit on the number of homes with PV is placed in the model under the assumption that renters and landlords are unlikely to install PV systems on rental units.
+LA has ~50% rental fraction</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nick Laws:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>function of ( NPV - INIT(NPV) )+incentive.
+Initial value of PV innovation rate set to 0.5% of regular customers per year (same as 2014 value found from permit data)
+Assumed to grow linearly to 5% when NPV reaches $10,000 greater than NPV in 2015
+(0.5% value estimated using Census values and reported PV installations by Souther California Edison)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function of NPV + incentive
+Assumed to be 0.1% of existing PV customers per year for a $2,000 NPV. 
+Grows linearly to 0.4% for NPV = $10,000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nick Laws:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Graphical function of NPV+incentive
+Battery innovation rate is assumed to be 
+0.1% of existing offgrid customers per year for the initial NPV. 
+Grows linearly to 0.5% for a $10,000 increase in NPV from the initial NPV.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nick Laws:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Graphical function of NPV + incentive
+Battery imitation rate is assumed to be 
+0.1% of existing PV customers per year for a $2,000 NPV. 
+Grows linearly to 0.4% for NPV = $10,000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nick Laws:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Graphical function of NPV+incentive
+Pv&amp;Battery innovation rate is assumed to be 
+0.1% of existing offgrid customers per year for zero NPV+incentive. 
+Grows linearly to 0.5% for a $10,000  NPV+incentive.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Graphical function of NPV + incentive
+PV&amp;Battery imitation rate is assumed to be 
+0.1% of existing PV customers per year for a $2,000 NPV. 
+Grows linearly to 0.4% for NPV = $10,000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+used for comparison plots</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+used for comparison plots</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+graphical function of (customers_with_PV+defectors)
+/ total_households
+Increases PV adoption through imitation as the number of homes with PV systems increases.
+Starts as 1 (no effect) with no PV homes. Grows linearly to 2 as all homes become PV homes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>these are time vectors, but we should not change them for each city? Perhaps have to switch to AUS dollars?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nick Laws</author>
+  </authors>
+  <commentList>
     <comment ref="I1" authorId="0">
       <text>
         <r>
@@ -962,7 +1425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="173">
   <si>
     <t>population growth rate</t>
   </si>
@@ -1492,7 +1955,14 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1614,119 +2084,123 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1735,13 +2209,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1772,7 +2246,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1783,26 +2257,26 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1817,8 +2291,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1829,20 +2303,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="89" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1930,8 +2409,12 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="89" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2263,7 +2746,7 @@
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="M2" sqref="M2:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3761,7 +4244,7 @@
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5255,14 +5738,1101 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:28" s="16" customFormat="1" ht="64" customHeight="1">
+      <c r="B1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="P1" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="S1" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="U1" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="V1" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" s="58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="16" customFormat="1" ht="18" customHeight="1">
+      <c r="B2">
+        <v>1448848</v>
+      </c>
+      <c r="C2">
+        <v>293639</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>7000</v>
+      </c>
+      <c r="F2">
+        <v>5694</v>
+      </c>
+      <c r="G2">
+        <v>32.4</v>
+      </c>
+      <c r="H2" s="63"/>
+      <c r="I2" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2" s="18">
+        <v>300</v>
+      </c>
+      <c r="N2" s="19">
+        <v>100</v>
+      </c>
+      <c r="O2" s="19">
+        <v>400</v>
+      </c>
+      <c r="P2" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="36">
+        <v>5.3900709219858204E-3</v>
+      </c>
+      <c r="R2" s="24">
+        <v>0</v>
+      </c>
+      <c r="S2" s="24">
+        <v>8.1560283687943296E-4</v>
+      </c>
+      <c r="T2" s="24">
+        <v>3.3444816053511699E-5</v>
+      </c>
+      <c r="U2" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="V2" s="24">
+        <v>6.6889632107023397E-5</v>
+      </c>
+      <c r="W2" s="29">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="X2" s="29">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="Y2" s="38">
+        <v>1</v>
+      </c>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="H3" s="64"/>
+      <c r="I3" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M3" s="19">
+        <v>300</v>
+      </c>
+      <c r="N3" s="14">
+        <v>100</v>
+      </c>
+      <c r="O3" s="14">
+        <v>400</v>
+      </c>
+      <c r="P3" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>8.6879432624113496E-3</v>
+      </c>
+      <c r="R3" s="25">
+        <v>5.0167224080267597E-4</v>
+      </c>
+      <c r="S3" s="25">
+        <v>1.3829787234042601E-3</v>
+      </c>
+      <c r="T3" s="25">
+        <v>3.3444816053511699E-4</v>
+      </c>
+      <c r="U3" s="25">
+        <v>1.4886731391585801E-3</v>
+      </c>
+      <c r="V3" s="25">
+        <v>2.6755852842809402E-4</v>
+      </c>
+      <c r="W3" s="9">
+        <v>0.28089999999999998</v>
+      </c>
+      <c r="X3" s="9">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="Y3" s="39">
+        <v>1.12380952380952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="I4" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M4" s="20">
+        <v>300</v>
+      </c>
+      <c r="N4" s="14">
+        <v>100</v>
+      </c>
+      <c r="O4" s="14">
+        <v>400</v>
+      </c>
+      <c r="P4" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>1.0638297872340399E-2</v>
+      </c>
+      <c r="R4" s="26">
+        <v>9.6989966555183996E-4</v>
+      </c>
+      <c r="S4" s="26">
+        <v>1.70212765957447E-3</v>
+      </c>
+      <c r="T4" s="26">
+        <v>7.6923076923076901E-4</v>
+      </c>
+      <c r="U4" s="26">
+        <v>1.94174757281553E-3</v>
+      </c>
+      <c r="V4" s="26">
+        <v>5.6856187290969904E-4</v>
+      </c>
+      <c r="W4" s="9">
+        <v>0.22259999999999999</v>
+      </c>
+      <c r="X4" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="Y4" s="40">
+        <v>1.2253968253968299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="I5" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M5" s="20">
+        <v>300</v>
+      </c>
+      <c r="N5" s="14">
+        <v>100</v>
+      </c>
+      <c r="O5" s="14">
+        <v>400</v>
+      </c>
+      <c r="P5" s="31">
+        <v>0.98936170212765995</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>1.24113475177305E-2</v>
+      </c>
+      <c r="R5" s="26">
+        <v>1.3712374581939799E-3</v>
+      </c>
+      <c r="S5" s="26">
+        <v>1.87943262411348E-3</v>
+      </c>
+      <c r="T5" s="26">
+        <v>1.10367892976589E-3</v>
+      </c>
+      <c r="U5" s="26">
+        <v>2.2330097087378598E-3</v>
+      </c>
+      <c r="V5" s="26">
+        <v>9.3645484949832799E-4</v>
+      </c>
+      <c r="W5" s="9">
+        <v>0.20979999999999999</v>
+      </c>
+      <c r="X5" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="Y5" s="40">
+        <v>1.35238095238095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="I6" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M6" s="21">
+        <v>300</v>
+      </c>
+      <c r="N6" s="14">
+        <v>100</v>
+      </c>
+      <c r="O6" s="14">
+        <v>400</v>
+      </c>
+      <c r="P6" s="29">
+        <v>0.97163120567375905</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>1.3829787234042599E-2</v>
+      </c>
+      <c r="R6" s="27">
+        <v>1.7391304347826101E-3</v>
+      </c>
+      <c r="S6" s="27">
+        <v>2.1985815602836899E-3</v>
+      </c>
+      <c r="T6" s="27">
+        <v>1.60535117056856E-3</v>
+      </c>
+      <c r="U6" s="27">
+        <v>2.5889967637540501E-3</v>
+      </c>
+      <c r="V6" s="27">
+        <v>1.3712374581939799E-3</v>
+      </c>
+      <c r="W6" s="4">
+        <v>0.19389999999999999</v>
+      </c>
+      <c r="X6" s="17">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="Y6" s="41">
+        <v>1.4539682539682499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M7" s="22">
+        <v>300</v>
+      </c>
+      <c r="N7" s="14">
+        <v>100</v>
+      </c>
+      <c r="O7" s="14">
+        <v>400</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0.95390070921985803</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>1.5957446808510599E-2</v>
+      </c>
+      <c r="R7" s="28">
+        <v>2.10702341137124E-3</v>
+      </c>
+      <c r="S7" s="28">
+        <v>2.5177304964538998E-3</v>
+      </c>
+      <c r="T7" s="28">
+        <v>2.0066889632107E-3</v>
+      </c>
+      <c r="U7" s="28">
+        <v>2.8478964401294502E-3</v>
+      </c>
+      <c r="V7" s="28">
+        <v>1.7725752508361201E-3</v>
+      </c>
+      <c r="W7" s="4">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Y7" s="42">
+        <v>1.5492063492063499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="I8" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M8" s="18">
+        <v>300</v>
+      </c>
+      <c r="N8" s="14">
+        <v>100</v>
+      </c>
+      <c r="O8" s="14">
+        <v>400</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0.91843971631205701</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>1.89716312056738E-2</v>
+      </c>
+      <c r="R8" s="24">
+        <v>2.4414715719063501E-3</v>
+      </c>
+      <c r="S8" s="24">
+        <v>2.9432624113475202E-3</v>
+      </c>
+      <c r="T8" s="24">
+        <v>2.5083612040133802E-3</v>
+      </c>
+      <c r="U8" s="24">
+        <v>3.20388349514563E-3</v>
+      </c>
+      <c r="V8" s="24">
+        <v>2.2408026755852801E-3</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0.1799</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="Y8" s="38">
+        <v>1.6317460317460299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="I9" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M9" s="18">
+        <v>300</v>
+      </c>
+      <c r="N9" s="14">
+        <v>100</v>
+      </c>
+      <c r="O9" s="14">
+        <v>400</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.879432624113475</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>2.2163120567375901E-2</v>
+      </c>
+      <c r="R9" s="24">
+        <v>2.9096989966555199E-3</v>
+      </c>
+      <c r="S9" s="24">
+        <v>3.43971631205674E-3</v>
+      </c>
+      <c r="T9" s="24">
+        <v>2.9765886287625399E-3</v>
+      </c>
+      <c r="U9" s="24">
+        <v>3.5922330097087401E-3</v>
+      </c>
+      <c r="V9" s="24">
+        <v>2.7090301003344498E-3</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0.17349999999999999</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0.505</v>
+      </c>
+      <c r="Y9" s="38">
+        <v>1.6952380952381001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="I10" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>300</v>
+      </c>
+      <c r="N10" s="14">
+        <v>100</v>
+      </c>
+      <c r="O10" s="14">
+        <v>400</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>2.4468085106383E-2</v>
+      </c>
+      <c r="R10" s="24">
+        <v>3.24414715719064E-3</v>
+      </c>
+      <c r="S10" s="24">
+        <v>4.1134751773049599E-3</v>
+      </c>
+      <c r="T10" s="24">
+        <v>3.3779264214046801E-3</v>
+      </c>
+      <c r="U10" s="24">
+        <v>4.1100323624595498E-3</v>
+      </c>
+      <c r="V10" s="24">
+        <v>3.17725752508361E-3</v>
+      </c>
+      <c r="W10" s="4">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="X10" s="4">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="Y10" s="38">
+        <v>1.7904761904761901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="I11" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M11" s="18">
+        <v>300</v>
+      </c>
+      <c r="N11" s="14">
+        <v>100</v>
+      </c>
+      <c r="O11" s="14">
+        <v>400</v>
+      </c>
+      <c r="P11" s="29">
+        <v>0.78723404255319196</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>2.73049645390071E-2</v>
+      </c>
+      <c r="R11" s="24">
+        <v>3.5785953177257502E-3</v>
+      </c>
+      <c r="S11" s="24">
+        <v>4.4680851063829798E-3</v>
+      </c>
+      <c r="T11" s="24">
+        <v>3.7792642140468198E-3</v>
+      </c>
+      <c r="U11" s="24">
+        <v>4.6601941747572801E-3</v>
+      </c>
+      <c r="V11" s="24">
+        <v>3.6454849498327802E-3</v>
+      </c>
+      <c r="W11" s="4">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="X11" s="4">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="Y11" s="38">
+        <v>1.89206349206349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="I12" s="65">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M12" s="18">
+        <v>300</v>
+      </c>
+      <c r="N12" s="14">
+        <v>100</v>
+      </c>
+      <c r="O12" s="14">
+        <v>400</v>
+      </c>
+      <c r="P12" s="29">
+        <v>0.70567375886524797</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>3.0496453900709201E-2</v>
+      </c>
+      <c r="R12" s="24">
+        <v>4.0133779264214103E-3</v>
+      </c>
+      <c r="S12" s="24">
+        <v>5.1063829787233997E-3</v>
+      </c>
+      <c r="T12" s="24">
+        <v>4.2809364548495E-3</v>
+      </c>
+      <c r="U12" s="24">
+        <v>5.2427184466019398E-3</v>
+      </c>
+      <c r="V12" s="24">
+        <v>4.0802675585284304E-3</v>
+      </c>
+      <c r="W12" s="4">
+        <v>0.15740000000000001</v>
+      </c>
+      <c r="X12" s="4">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="Y12" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
+      <c r="M13" s="18">
+        <v>300</v>
+      </c>
+      <c r="N13" s="14">
+        <v>100</v>
+      </c>
+      <c r="O13" s="14">
+        <v>400</v>
+      </c>
+      <c r="P13" s="29">
+        <v>0.62411347517730498</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>3.2269503546099303E-2</v>
+      </c>
+      <c r="W13" s="4">
+        <v>0.152</v>
+      </c>
+      <c r="X13" s="4">
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="M14" s="18">
+        <v>300</v>
+      </c>
+      <c r="N14" s="14">
+        <v>100</v>
+      </c>
+      <c r="O14" s="14">
+        <v>400</v>
+      </c>
+      <c r="P14" s="29">
+        <v>0.46099290780141799</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>3.5106382978723399E-2</v>
+      </c>
+      <c r="W14" s="4">
+        <v>0.153</v>
+      </c>
+      <c r="X14" s="4">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28">
+      <c r="M15" s="18">
+        <v>300</v>
+      </c>
+      <c r="N15" s="14">
+        <v>100</v>
+      </c>
+      <c r="O15" s="14">
+        <v>400</v>
+      </c>
+      <c r="P15" s="29">
+        <v>0.28723404255319201</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>3.7411347517730502E-2</v>
+      </c>
+      <c r="W15" s="4">
+        <v>0.152</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
+      <c r="M16" s="18">
+        <v>300</v>
+      </c>
+      <c r="N16" s="14">
+        <v>100</v>
+      </c>
+      <c r="O16" s="14">
+        <v>400</v>
+      </c>
+      <c r="P16" s="29">
+        <v>0.184397163120567</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>3.9716312056737597E-2</v>
+      </c>
+      <c r="W16" s="4">
+        <v>0.15090000000000001</v>
+      </c>
+      <c r="X16" s="4">
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="13:24">
+      <c r="M17" s="18">
+        <v>300</v>
+      </c>
+      <c r="N17" s="14">
+        <v>100</v>
+      </c>
+      <c r="O17" s="14">
+        <v>400</v>
+      </c>
+      <c r="P17" s="29">
+        <v>8.5106382978723402E-2</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>4.3262411347517703E-2</v>
+      </c>
+      <c r="W17" s="4">
+        <v>0.14979999999999999</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="18" spans="13:24">
+      <c r="M18" s="18">
+        <v>300</v>
+      </c>
+      <c r="N18" s="14">
+        <v>100</v>
+      </c>
+      <c r="O18" s="14">
+        <v>400</v>
+      </c>
+      <c r="P18" s="29">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>4.4858156028368797E-2</v>
+      </c>
+      <c r="W18" s="4">
+        <v>0.1487</v>
+      </c>
+      <c r="X18" s="4">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="19" spans="13:24">
+      <c r="M19" s="18">
+        <v>300</v>
+      </c>
+      <c r="N19" s="14">
+        <v>100</v>
+      </c>
+      <c r="O19" s="14">
+        <v>400</v>
+      </c>
+      <c r="P19" s="29">
+        <v>2.1276595744680899E-2</v>
+      </c>
+      <c r="Q19" s="23">
+        <v>4.6808510638297898E-2</v>
+      </c>
+      <c r="W19" s="4">
+        <v>0.1479</v>
+      </c>
+      <c r="X19" s="4">
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="20" spans="13:24">
+      <c r="M20" s="18">
+        <v>300</v>
+      </c>
+      <c r="N20" s="14">
+        <v>100</v>
+      </c>
+      <c r="O20" s="14">
+        <v>400</v>
+      </c>
+      <c r="P20" s="29">
+        <v>3.54609929078014E-3</v>
+      </c>
+      <c r="Q20" s="23">
+        <v>4.8936170212766E-2</v>
+      </c>
+      <c r="W20" s="4">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="X20" s="4">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="21" spans="13:24">
+      <c r="M21" s="18">
+        <v>300</v>
+      </c>
+      <c r="N21" s="14">
+        <v>100</v>
+      </c>
+      <c r="O21" s="14">
+        <v>400</v>
+      </c>
+      <c r="P21" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="W21" s="4">
+        <v>0.14369999999999999</v>
+      </c>
+      <c r="X21" s="4">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="13:24">
+      <c r="M22" s="18">
+        <v>300</v>
+      </c>
+      <c r="N22" s="14">
+        <v>100</v>
+      </c>
+      <c r="O22" s="14">
+        <v>400</v>
+      </c>
+      <c r="P22" s="29">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="23">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="W22" s="4">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="X22" s="4">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="13:24">
+      <c r="M23" s="18">
+        <v>300</v>
+      </c>
+      <c r="N23" s="14">
+        <v>100</v>
+      </c>
+      <c r="O23" s="14">
+        <v>400</v>
+      </c>
+      <c r="W23" s="4">
+        <v>0.1419</v>
+      </c>
+      <c r="X23" s="4">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="13:24">
+      <c r="M24" s="18">
+        <v>300</v>
+      </c>
+      <c r="N24" s="14">
+        <v>100</v>
+      </c>
+      <c r="O24" s="14">
+        <v>400</v>
+      </c>
+      <c r="W24" s="4">
+        <v>0.14169999999999999</v>
+      </c>
+      <c r="X24" s="4">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="13:24">
+      <c r="M25" s="18">
+        <v>300</v>
+      </c>
+      <c r="N25" s="14">
+        <v>100</v>
+      </c>
+      <c r="O25" s="14">
+        <v>400</v>
+      </c>
+      <c r="W25" s="4">
+        <v>0.1414</v>
+      </c>
+      <c r="X25" s="4">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="13:24">
+      <c r="M26" s="18">
+        <v>300</v>
+      </c>
+      <c r="N26" s="14">
+        <v>100</v>
+      </c>
+      <c r="O26" s="14">
+        <v>400</v>
+      </c>
+      <c r="W26" s="4">
+        <v>0.14119999999999999</v>
+      </c>
+      <c r="X26" s="4">
+        <v>0.35699999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="13:24">
+      <c r="M27" s="18">
+        <v>300</v>
+      </c>
+      <c r="N27" s="14">
+        <v>100</v>
+      </c>
+      <c r="O27" s="14">
+        <v>400</v>
+      </c>
+      <c r="W27" s="4">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="X27" s="4">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="13:24">
+      <c r="M28" s="18">
+        <v>300</v>
+      </c>
+      <c r="N28" s="14">
+        <v>100</v>
+      </c>
+      <c r="O28" s="14">
+        <v>400</v>
+      </c>
+      <c r="W28" s="4">
+        <v>0.14069999999999999</v>
+      </c>
+      <c r="X28" s="4">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="13:24">
+      <c r="M29" s="18">
+        <v>300</v>
+      </c>
+      <c r="N29" s="14">
+        <v>100</v>
+      </c>
+      <c r="O29" s="14">
+        <v>400</v>
+      </c>
+      <c r="W29" s="4">
+        <v>0.14050000000000001</v>
+      </c>
+      <c r="X29" s="4">
+        <v>0.35099999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="13:24">
+      <c r="M30" s="18">
+        <v>300</v>
+      </c>
+      <c r="N30" s="14">
+        <v>100</v>
+      </c>
+      <c r="O30" s="14">
+        <v>400</v>
+      </c>
+      <c r="W30" s="4">
+        <v>0.14019999999999999</v>
+      </c>
+      <c r="X30" s="4">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="31" spans="13:24">
+      <c r="M31" s="18">
+        <v>300</v>
+      </c>
+      <c r="N31" s="14">
+        <v>100</v>
+      </c>
+      <c r="O31" s="14">
+        <v>400</v>
+      </c>
+      <c r="W31" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X31" s="4">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="13:24">
+      <c r="M32" s="18">
+        <v>300</v>
+      </c>
+      <c r="N32" s="14">
+        <v>100</v>
+      </c>
+      <c r="O32" s="14">
+        <v>400</v>
+      </c>
+      <c r="W32" s="4">
+        <v>0.13980000000000001</v>
+      </c>
+      <c r="X32" s="4">
+        <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="13:24">
+      <c r="M33" s="18">
+        <v>300</v>
+      </c>
+      <c r="N33" s="14">
+        <v>100</v>
+      </c>
+      <c r="O33" s="14">
+        <v>400</v>
+      </c>
+      <c r="W33" s="4">
+        <v>0.13950000000000001</v>
+      </c>
+      <c r="X33" s="4">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="13:24">
+      <c r="M34" s="18">
+        <v>300</v>
+      </c>
+      <c r="N34" s="14">
+        <v>100</v>
+      </c>
+      <c r="O34" s="14">
+        <v>400</v>
+      </c>
+      <c r="W34" s="4">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="X34" s="4">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="13:24">
+      <c r="M35" s="18">
+        <v>300</v>
+      </c>
+      <c r="N35" s="14">
+        <v>100</v>
+      </c>
+      <c r="O35" s="14">
+        <v>400</v>
+      </c>
+      <c r="W35" s="4">
+        <v>0.1391</v>
+      </c>
+      <c r="X35" s="4">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="36" spans="13:24">
+      <c r="M36" s="18">
+        <v>300</v>
+      </c>
+      <c r="N36" s="14">
+        <v>100</v>
+      </c>
+      <c r="O36" s="14">
+        <v>400</v>
+      </c>
+      <c r="W36" s="4">
+        <v>0.13880000000000001</v>
+      </c>
+      <c r="X36" s="4">
+        <v>0.33900000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="13:24">
+      <c r="M37" s="18">
+        <v>300</v>
+      </c>
+      <c r="N37" s="14">
+        <v>100</v>
+      </c>
+      <c r="O37" s="14">
+        <v>400</v>
+      </c>
+      <c r="W37" s="4">
+        <v>0.1386</v>
+      </c>
+      <c r="X37" s="4">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="13:24">
+      <c r="M38" s="18">
+        <v>300</v>
+      </c>
+      <c r="N38" s="14">
+        <v>100</v>
+      </c>
+      <c r="O38" s="14">
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5275,7 +6845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
drain slowing functions were not defined correctly and they allowed zero grid customers. I have fixed this issue in all models and they can now handle all extreme values. added location folders to the github 'Model' folder.  Each location folder contains two versions of each business model. One version is 'switched' and uses the interface to run the models with our sensitivity variables. The other versions contain no interface functions so that they can be used for running the sensitivity analyses.
also added a dummy variable for direct PV use  in the models that do not use this variable so that there will be no warning with this item as well.
</commit_message>
<xml_diff>
--- a/Model/Data/import.xlsx
+++ b/Model/Data/import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="15700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="15700" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="1" r:id="rId1"/>
@@ -2173,7 +2173,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -2338,7 +2338,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2429,6 +2429,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2495,15 +2497,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2612,7 +2614,7 @@
       <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2715,6 +2717,8 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="89" builtinId="5"/>
@@ -3056,7 +3060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -7524,8 +7528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7642,25 +7646,25 @@
         <v>5000</v>
       </c>
       <c r="C3">
-        <v>20000</v>
+        <v>5000</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J3" s="66">
         <v>1</v>
@@ -7692,25 +7696,25 @@
         <v>10000</v>
       </c>
       <c r="C4" s="13">
-        <v>40000</v>
+        <v>10000</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J4" s="73">
         <v>1</v>

</xml_diff>

<commit_message>
work in progress on version 4 of paper. See death spiral paper notes.rtfdin Kite drive for detailed notes
</commit_message>
<xml_diff>
--- a/Model/Data/import.xlsx
+++ b/Model/Data/import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="15700" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LA" sheetId="1" r:id="rId1"/>
@@ -1378,6 +1378,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Laws:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4kW system production from Kamau reference.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="N2" authorId="0">
       <text>
         <r>
@@ -1649,7 +1673,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="173">
   <si>
     <t>population growth rate</t>
   </si>
@@ -2165,6 +2189,9 @@
   </si>
   <si>
     <t>(estimated)</t>
+  </si>
+  <si>
+    <t>use 1.25*5700?</t>
   </si>
 </sst>
 </file>
@@ -2447,7 +2474,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2613,6 +2640,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3061,7 +3089,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4575,7 +4603,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4703,8 +4731,8 @@
       <c r="H2" s="34">
         <v>0.1246</v>
       </c>
-      <c r="I2" s="10">
-        <v>0.10100000000000001</v>
+      <c r="I2" s="77">
+        <v>6.2300000000000001E-2</v>
       </c>
       <c r="J2" s="23">
         <v>8.0000000000000002E-3</v>
@@ -6088,8 +6116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6190,7 +6218,7 @@
       <c r="F2">
         <v>7000</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="54">
         <v>5694</v>
       </c>
       <c r="H2" s="22">
@@ -6312,6 +6340,9 @@
       </c>
     </row>
     <row r="4" spans="1:29">
+      <c r="G4" t="s">
+        <v>172</v>
+      </c>
       <c r="J4" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -6365,6 +6396,10 @@
       </c>
     </row>
     <row r="5" spans="1:29">
+      <c r="G5">
+        <f>1.25*5700</f>
+        <v>7125</v>
+      </c>
       <c r="J5" s="60">
         <v>1.7999999999999999E-2</v>
       </c>
@@ -7528,7 +7563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>